<commit_message>
Committing the modified files as well as adding new files.
Committing the modified files as well as adding new files.
</commit_message>
<xml_diff>
--- a/Technical things.xlsx
+++ b/Technical things.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\03-29-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A7C7F3-7F83-487A-B164-D50A8D9D5C64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD93224-BCFF-4EDB-9390-3D34DA398AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Sr No.</t>
   </si>
@@ -443,7 +443,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +553,9 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2">

</xml_diff>